<commit_message>
Atualização da Documentacao Tabela LN
</commit_message>
<xml_diff>
--- a/Documentação/Tabelas_LN/zncmg015-Cancelamentos Cartao Credito.xlsx
+++ b/Documentação/Tabelas_LN/zncmg015-Cancelamentos Cartao Credito.xlsx
@@ -2849,11 +2849,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048575 E2:E1048575">
-      <formula1>ttyeno</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048575">
       <formula1>ttadv.type</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048575 L2:L1048575">
+      <formula1>ttyeno</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>